<commit_message>
starting to fix DRC errors
</commit_message>
<xml_diff>
--- a/BabyHuey.xlsx
+++ b/BabyHuey.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Tristan/GitRepos/amps/HiFi-BabyHuey/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{1A5E430F-5454-9E4F-B044-9B4DDA98AEDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4D3286B-4C35-D145-BC30-3BE2492821AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16620"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BabyHuey" sheetId="1" r:id="rId1"/>
+    <sheet name="BabyHuey (2)" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="595" uniqueCount="228">
   <si>
     <t>Source:</t>
   </si>
@@ -640,12 +641,87 @@
   </si>
   <si>
     <t>10r 2W</t>
+  </si>
+  <si>
+    <t>/Users/Tristan/GitRepos/amps/HiFi-BabyHuey/BabyHuey.kicad_sch</t>
+  </si>
+  <si>
+    <t>Wednesday, 29 December 2021 at 20:12:28</t>
+  </si>
+  <si>
+    <t>Eeschema (6.0.0-0)</t>
+  </si>
+  <si>
+    <t>/Applications/KiCad/KiCad.app/Contents/SharedSupport/plugins/bom_csv_grouped_by_value_with_fp.py</t>
+  </si>
+  <si>
+    <t>C_Polarized</t>
+  </si>
+  <si>
+    <t>Polarized capacitor</t>
+  </si>
+  <si>
+    <t>Capacitor_THT:CP_Radial_D12.5mm_P5.00mm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C205, C210, C307, C407, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">C206, C211, C304, C305, C404, C405, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">C207, C306, C406, </t>
+  </si>
+  <si>
+    <t>Capacitor_THT:CP_Radial_D5.0mm_P2.50mm</t>
+  </si>
+  <si>
+    <t>Capacitor_THT:C_Rect_L26.5mm_W8.5mm_P22.50mm_MKS4</t>
+  </si>
+  <si>
+    <t>Diode_THT:D_DO-35_SOD27_P7.62mm_Horizontal</t>
+  </si>
+  <si>
+    <t>Resistor_THT:R_Axial_Power_L25.0mm_W9.0mm_P30.48mm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R201, R202, R208, R209, R317, R318, R319, R320, R417, R418, R419, R420, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">R203, R205, R314, R414, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">R204, R206, R312, R313, R412, R413, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">R207, R212, R214, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">R210, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">R213, R305, R405, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">R215, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RV201, RV302, RV303, RV402, RV403, </t>
+  </si>
+  <si>
+    <t>R_Potentiometer_Trim</t>
+  </si>
+  <si>
+    <t>Trim-potentiometer</t>
+  </si>
+  <si>
+    <t>https://cdn-reichelt.de/documents/datenblatt/C151/RND_205-00023_DB_EN.pdf</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1493,11 +1569,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2010,6 +2086,9 @@
       <c r="F25" t="s">
         <v>80</v>
       </c>
+      <c r="I25" t="s">
+        <v>227</v>
+      </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
@@ -2698,6 +2777,1162 @@
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>173</v>
+      </c>
+      <c r="B60">
+        <v>4</v>
+      </c>
+      <c r="C60" t="s">
+        <v>174</v>
+      </c>
+      <c r="D60" t="s">
+        <v>174</v>
+      </c>
+      <c r="E60" t="s">
+        <v>175</v>
+      </c>
+      <c r="F60" t="s">
+        <v>176</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7196C216-68C7-3145-A63F-CDDBCF57341C}">
+  <dimension ref="A1:G60"/>
+  <sheetViews>
+    <sheetView topLeftCell="A34" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" t="s">
+        <v>207</v>
+      </c>
+      <c r="E8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" t="s">
+        <v>207</v>
+      </c>
+      <c r="E9" t="s">
+        <v>209</v>
+      </c>
+      <c r="F9" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>210</v>
+      </c>
+      <c r="B10">
+        <v>4</v>
+      </c>
+      <c r="C10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" t="s">
+        <v>207</v>
+      </c>
+      <c r="E10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>211</v>
+      </c>
+      <c r="B11">
+        <v>6</v>
+      </c>
+      <c r="C11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" t="s">
+        <v>207</v>
+      </c>
+      <c r="E11" t="s">
+        <v>209</v>
+      </c>
+      <c r="F11" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>212</v>
+      </c>
+      <c r="B12">
+        <v>3</v>
+      </c>
+      <c r="C12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" t="s">
+        <v>207</v>
+      </c>
+      <c r="E12" t="s">
+        <v>213</v>
+      </c>
+      <c r="F12" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" t="s">
+        <v>207</v>
+      </c>
+      <c r="E13" t="s">
+        <v>27</v>
+      </c>
+      <c r="F13" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" t="s">
+        <v>207</v>
+      </c>
+      <c r="E14" t="s">
+        <v>39</v>
+      </c>
+      <c r="F14" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15" t="s">
+        <v>41</v>
+      </c>
+      <c r="D15" t="s">
+        <v>207</v>
+      </c>
+      <c r="E15" t="s">
+        <v>39</v>
+      </c>
+      <c r="F15" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16" t="s">
+        <v>43</v>
+      </c>
+      <c r="D16" t="s">
+        <v>18</v>
+      </c>
+      <c r="E16" t="s">
+        <v>44</v>
+      </c>
+      <c r="F16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17">
+        <v>4</v>
+      </c>
+      <c r="C17" t="s">
+        <v>46</v>
+      </c>
+      <c r="D17" t="s">
+        <v>18</v>
+      </c>
+      <c r="E17" t="s">
+        <v>214</v>
+      </c>
+      <c r="F17" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>48</v>
+      </c>
+      <c r="B18">
+        <v>4</v>
+      </c>
+      <c r="C18" t="s">
+        <v>49</v>
+      </c>
+      <c r="D18" t="s">
+        <v>50</v>
+      </c>
+      <c r="E18" t="s">
+        <v>51</v>
+      </c>
+      <c r="F18" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>53</v>
+      </c>
+      <c r="B19">
+        <v>8</v>
+      </c>
+      <c r="C19" t="s">
+        <v>54</v>
+      </c>
+      <c r="D19" t="s">
+        <v>50</v>
+      </c>
+      <c r="E19" t="s">
+        <v>55</v>
+      </c>
+      <c r="F19" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>56</v>
+      </c>
+      <c r="B20">
+        <v>6</v>
+      </c>
+      <c r="C20" t="s">
+        <v>57</v>
+      </c>
+      <c r="D20" t="s">
+        <v>58</v>
+      </c>
+      <c r="E20" t="s">
+        <v>215</v>
+      </c>
+      <c r="F20" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>60</v>
+      </c>
+      <c r="B21">
+        <v>4</v>
+      </c>
+      <c r="C21" t="s">
+        <v>61</v>
+      </c>
+      <c r="D21" t="s">
+        <v>62</v>
+      </c>
+      <c r="E21" t="s">
+        <v>63</v>
+      </c>
+      <c r="F21" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>65</v>
+      </c>
+      <c r="B22">
+        <v>2</v>
+      </c>
+      <c r="C22" t="s">
+        <v>66</v>
+      </c>
+      <c r="D22" t="s">
+        <v>67</v>
+      </c>
+      <c r="E22" t="s">
+        <v>68</v>
+      </c>
+      <c r="F22" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>69</v>
+      </c>
+      <c r="B23">
+        <v>10</v>
+      </c>
+      <c r="C23" t="s">
+        <v>70</v>
+      </c>
+      <c r="D23" t="s">
+        <v>70</v>
+      </c>
+      <c r="E23" t="s">
+        <v>71</v>
+      </c>
+      <c r="F23" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>73</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24" t="s">
+        <v>74</v>
+      </c>
+      <c r="D24" t="s">
+        <v>74</v>
+      </c>
+      <c r="E24" t="s">
+        <v>75</v>
+      </c>
+      <c r="F24" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>77</v>
+      </c>
+      <c r="B25">
+        <v>2</v>
+      </c>
+      <c r="C25" t="s">
+        <v>78</v>
+      </c>
+      <c r="D25" t="s">
+        <v>78</v>
+      </c>
+      <c r="E25" t="s">
+        <v>79</v>
+      </c>
+      <c r="F25" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>81</v>
+      </c>
+      <c r="B26">
+        <v>8</v>
+      </c>
+      <c r="C26" t="s">
+        <v>82</v>
+      </c>
+      <c r="D26" t="s">
+        <v>82</v>
+      </c>
+      <c r="E26" t="s">
+        <v>83</v>
+      </c>
+      <c r="F26" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>85</v>
+      </c>
+      <c r="B27">
+        <v>2</v>
+      </c>
+      <c r="C27" t="s">
+        <v>86</v>
+      </c>
+      <c r="D27" t="s">
+        <v>86</v>
+      </c>
+      <c r="E27" t="s">
+        <v>87</v>
+      </c>
+      <c r="F27" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>89</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28" t="s">
+        <v>90</v>
+      </c>
+      <c r="D28" t="s">
+        <v>91</v>
+      </c>
+      <c r="E28" t="s">
+        <v>92</v>
+      </c>
+      <c r="F28" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>94</v>
+      </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
+      <c r="C29" t="s">
+        <v>95</v>
+      </c>
+      <c r="D29" t="s">
+        <v>96</v>
+      </c>
+      <c r="E29" t="s">
+        <v>92</v>
+      </c>
+      <c r="F29" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>98</v>
+      </c>
+      <c r="B30">
+        <v>12</v>
+      </c>
+      <c r="C30" t="s">
+        <v>99</v>
+      </c>
+      <c r="D30" t="s">
+        <v>100</v>
+      </c>
+      <c r="E30" t="s">
+        <v>101</v>
+      </c>
+      <c r="F30" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>103</v>
+      </c>
+      <c r="B31">
+        <v>4</v>
+      </c>
+      <c r="C31" t="s">
+        <v>104</v>
+      </c>
+      <c r="D31" t="s">
+        <v>91</v>
+      </c>
+      <c r="E31" t="s">
+        <v>105</v>
+      </c>
+      <c r="F31" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>106</v>
+      </c>
+      <c r="B32">
+        <v>1</v>
+      </c>
+      <c r="C32" t="s">
+        <v>107</v>
+      </c>
+      <c r="D32" t="s">
+        <v>108</v>
+      </c>
+      <c r="E32" t="s">
+        <v>216</v>
+      </c>
+      <c r="F32" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>217</v>
+      </c>
+      <c r="B33">
+        <v>12</v>
+      </c>
+      <c r="C33" t="s">
+        <v>112</v>
+      </c>
+      <c r="D33" t="s">
+        <v>108</v>
+      </c>
+      <c r="E33" t="s">
+        <v>113</v>
+      </c>
+      <c r="F33" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>218</v>
+      </c>
+      <c r="B34">
+        <v>4</v>
+      </c>
+      <c r="C34" t="s">
+        <v>117</v>
+      </c>
+      <c r="D34" t="s">
+        <v>108</v>
+      </c>
+      <c r="E34" t="s">
+        <v>113</v>
+      </c>
+      <c r="F34" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>219</v>
+      </c>
+      <c r="B35">
+        <v>6</v>
+      </c>
+      <c r="C35" t="s">
+        <v>119</v>
+      </c>
+      <c r="D35" t="s">
+        <v>108</v>
+      </c>
+      <c r="E35" t="s">
+        <v>113</v>
+      </c>
+      <c r="F35" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>220</v>
+      </c>
+      <c r="B36">
+        <v>3</v>
+      </c>
+      <c r="C36" t="s">
+        <v>121</v>
+      </c>
+      <c r="D36" t="s">
+        <v>108</v>
+      </c>
+      <c r="E36" t="s">
+        <v>113</v>
+      </c>
+      <c r="F36" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>221</v>
+      </c>
+      <c r="B37">
+        <v>1</v>
+      </c>
+      <c r="C37" t="s">
+        <v>123</v>
+      </c>
+      <c r="D37" t="s">
+        <v>108</v>
+      </c>
+      <c r="E37" t="s">
+        <v>113</v>
+      </c>
+      <c r="F37" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>122</v>
+      </c>
+      <c r="B38">
+        <v>1</v>
+      </c>
+      <c r="C38" t="s">
+        <v>125</v>
+      </c>
+      <c r="D38" t="s">
+        <v>108</v>
+      </c>
+      <c r="E38" t="s">
+        <v>113</v>
+      </c>
+      <c r="F38" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>222</v>
+      </c>
+      <c r="B39">
+        <v>3</v>
+      </c>
+      <c r="C39" t="s">
+        <v>127</v>
+      </c>
+      <c r="D39" t="s">
+        <v>108</v>
+      </c>
+      <c r="E39" t="s">
+        <v>113</v>
+      </c>
+      <c r="F39" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>223</v>
+      </c>
+      <c r="B40">
+        <v>1</v>
+      </c>
+      <c r="C40" t="s">
+        <v>115</v>
+      </c>
+      <c r="D40" t="s">
+        <v>108</v>
+      </c>
+      <c r="E40" t="s">
+        <v>113</v>
+      </c>
+      <c r="F40" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>128</v>
+      </c>
+      <c r="B41">
+        <v>2</v>
+      </c>
+      <c r="C41" t="s">
+        <v>43</v>
+      </c>
+      <c r="D41" t="s">
+        <v>108</v>
+      </c>
+      <c r="E41" t="s">
+        <v>113</v>
+      </c>
+      <c r="F41" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>129</v>
+      </c>
+      <c r="B42">
+        <v>2</v>
+      </c>
+      <c r="C42" t="s">
+        <v>130</v>
+      </c>
+      <c r="D42" t="s">
+        <v>108</v>
+      </c>
+      <c r="E42" t="s">
+        <v>113</v>
+      </c>
+      <c r="F42" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>131</v>
+      </c>
+      <c r="B43">
+        <v>2</v>
+      </c>
+      <c r="C43" t="s">
+        <v>132</v>
+      </c>
+      <c r="D43" t="s">
+        <v>108</v>
+      </c>
+      <c r="E43" t="s">
+        <v>113</v>
+      </c>
+      <c r="F43" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>133</v>
+      </c>
+      <c r="B44">
+        <v>2</v>
+      </c>
+      <c r="C44" t="s">
+        <v>134</v>
+      </c>
+      <c r="D44" t="s">
+        <v>108</v>
+      </c>
+      <c r="E44" t="s">
+        <v>113</v>
+      </c>
+      <c r="F44" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>135</v>
+      </c>
+      <c r="B45">
+        <v>12</v>
+      </c>
+      <c r="C45" t="s">
+        <v>136</v>
+      </c>
+      <c r="D45" t="s">
+        <v>108</v>
+      </c>
+      <c r="E45" t="s">
+        <v>113</v>
+      </c>
+      <c r="F45" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>137</v>
+      </c>
+      <c r="B46">
+        <v>4</v>
+      </c>
+      <c r="C46" t="s">
+        <v>138</v>
+      </c>
+      <c r="D46" t="s">
+        <v>108</v>
+      </c>
+      <c r="E46" t="s">
+        <v>139</v>
+      </c>
+      <c r="F46" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>140</v>
+      </c>
+      <c r="B47">
+        <v>4</v>
+      </c>
+      <c r="C47" t="s">
+        <v>141</v>
+      </c>
+      <c r="D47" t="s">
+        <v>108</v>
+      </c>
+      <c r="E47" t="s">
+        <v>113</v>
+      </c>
+      <c r="F47" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>142</v>
+      </c>
+      <c r="B48">
+        <v>4</v>
+      </c>
+      <c r="C48" t="s">
+        <v>143</v>
+      </c>
+      <c r="D48" t="s">
+        <v>108</v>
+      </c>
+      <c r="E48" t="s">
+        <v>113</v>
+      </c>
+      <c r="F48" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>144</v>
+      </c>
+      <c r="B49">
+        <v>2</v>
+      </c>
+      <c r="C49" t="s">
+        <v>145</v>
+      </c>
+      <c r="D49" t="s">
+        <v>108</v>
+      </c>
+      <c r="E49" t="s">
+        <v>139</v>
+      </c>
+      <c r="F49" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>146</v>
+      </c>
+      <c r="B50">
+        <v>4</v>
+      </c>
+      <c r="C50" t="s">
+        <v>147</v>
+      </c>
+      <c r="D50" t="s">
+        <v>108</v>
+      </c>
+      <c r="E50" t="s">
+        <v>139</v>
+      </c>
+      <c r="F50" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>148</v>
+      </c>
+      <c r="B51">
+        <v>4</v>
+      </c>
+      <c r="C51" t="s">
+        <v>149</v>
+      </c>
+      <c r="D51" t="s">
+        <v>108</v>
+      </c>
+      <c r="E51" t="s">
+        <v>113</v>
+      </c>
+      <c r="F51" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>150</v>
+      </c>
+      <c r="B52">
+        <v>4</v>
+      </c>
+      <c r="C52" t="s">
+        <v>151</v>
+      </c>
+      <c r="D52" t="s">
+        <v>108</v>
+      </c>
+      <c r="E52" t="s">
+        <v>139</v>
+      </c>
+      <c r="F52" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>152</v>
+      </c>
+      <c r="B53">
+        <v>4</v>
+      </c>
+      <c r="C53" t="s">
+        <v>153</v>
+      </c>
+      <c r="D53" t="s">
+        <v>108</v>
+      </c>
+      <c r="E53" t="s">
+        <v>113</v>
+      </c>
+      <c r="F53" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>154</v>
+      </c>
+      <c r="B54">
+        <v>2</v>
+      </c>
+      <c r="C54" t="s">
+        <v>202</v>
+      </c>
+      <c r="D54" t="s">
+        <v>108</v>
+      </c>
+      <c r="E54" t="s">
+        <v>139</v>
+      </c>
+      <c r="F54" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>224</v>
+      </c>
+      <c r="B55">
+        <v>5</v>
+      </c>
+      <c r="C55" t="s">
+        <v>159</v>
+      </c>
+      <c r="D55" t="s">
+        <v>225</v>
+      </c>
+      <c r="E55" t="s">
+        <v>157</v>
+      </c>
+      <c r="F55" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>155</v>
+      </c>
+      <c r="B56">
+        <v>2</v>
+      </c>
+      <c r="C56" t="s">
+        <v>134</v>
+      </c>
+      <c r="D56" t="s">
+        <v>225</v>
+      </c>
+      <c r="E56" t="s">
+        <v>157</v>
+      </c>
+      <c r="F56" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>160</v>
+      </c>
+      <c r="B57">
+        <v>1</v>
+      </c>
+      <c r="C57" t="s">
+        <v>161</v>
+      </c>
+      <c r="D57" t="s">
+        <v>162</v>
+      </c>
+      <c r="E57" t="s">
+        <v>163</v>
+      </c>
+      <c r="F57" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>165</v>
+      </c>
+      <c r="B58">
+        <v>10</v>
+      </c>
+      <c r="C58" t="s">
+        <v>166</v>
+      </c>
+      <c r="D58" t="s">
+        <v>166</v>
+      </c>
+      <c r="E58" t="s">
+        <v>167</v>
+      </c>
+      <c r="F58" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>169</v>
+      </c>
+      <c r="B59">
+        <v>2</v>
+      </c>
+      <c r="C59" t="s">
+        <v>170</v>
+      </c>
+      <c r="D59" t="s">
+        <v>170</v>
+      </c>
+      <c r="E59" t="s">
+        <v>171</v>
+      </c>
+      <c r="F59" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>173</v>
       </c>

</xml_diff>

<commit_message>
adding in humdinger, tidying tracks
</commit_message>
<xml_diff>
--- a/BabyHuey.xlsx
+++ b/BabyHuey.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Tristan/GitRepos/HiFi-BabyHuey/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D232D9C7-7B39-0449-8819-81FFFB4BB1C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17CEFB9F-11EE-2344-B7C3-BDC9F1391C4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1589,8 +1589,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB340298-E73E-9A41-B0B6-F93061A8A872}">
   <dimension ref="A1:N66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F61" sqref="F61"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="K52" sqref="K52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3106,8 +3106,7 @@
         <v>3339P-1-501LF</v>
       </c>
       <c r="K51">
-        <f t="shared" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
update BoM, files for initial release
</commit_message>
<xml_diff>
--- a/BabyHuey.xlsx
+++ b/BabyHuey.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Tristan/GitRepos/HiFi-BabyHuey/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17CEFB9F-11EE-2344-B7C3-BDC9F1391C4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{644E586E-9827-3543-9093-3AD3B8C6A152}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="27960" windowHeight="16620" xr2:uid="{D9555A60-0B69-E04A-896F-B8CB5E71D4B1}"/>
   </bookViews>
   <sheets>
-    <sheet name="BabyHueyMaster" sheetId="3" r:id="rId1"/>
-    <sheet name="Mouser" sheetId="4" r:id="rId2"/>
+    <sheet name="BabyHuey" sheetId="5" r:id="rId1"/>
+    <sheet name="OLD-&gt;" sheetId="6" r:id="rId2"/>
+    <sheet name="Mouser" sheetId="4" r:id="rId3"/>
+    <sheet name="BabyHueyMaster" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="745" uniqueCount="265">
   <si>
     <t>Source:</t>
   </si>
@@ -283,9 +285,6 @@
     <t>Resistor_THT:R_Axial_DIN0207_L6.3mm_D2.5mm_P10.16mm_Horizontal</t>
   </si>
   <si>
-    <t>TBD</t>
-  </si>
-  <si>
     <t>22k</t>
   </si>
   <si>
@@ -517,9 +516,6 @@
     <t xml:space="preserve">R213, R305, R405, </t>
   </si>
   <si>
-    <t xml:space="preserve">R215, </t>
-  </si>
-  <si>
     <t xml:space="preserve">RV201, RV302, RV303, RV402, RV403, </t>
   </si>
   <si>
@@ -746,6 +742,93 @@
   </si>
   <si>
     <t>ECA-1EHG470I</t>
+  </si>
+  <si>
+    <t>Sunday, 09 January 2022 at 17:24:33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R201, R203, R314, R414, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">R202, R204, R312, R313, R412, R413, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">R205, R210, R212, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">R206, R207, R317, R318, R319, R320, R417, R418, R419, R420, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">R208, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">R209, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">R211, R305, R405, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RV201, RV302, RV402, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RV202, RV303, RV304, RV403, RV404, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">U301, U401, </t>
+  </si>
+  <si>
+    <t>ECC83</t>
+  </si>
+  <si>
+    <t>TC Valves:VALVE-ECC-83-1-TC</t>
+  </si>
+  <si>
+    <t>double triode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U302, U303, U402, U403, </t>
+  </si>
+  <si>
+    <t>EL34</t>
+  </si>
+  <si>
+    <t>TC Valves:Octal</t>
+  </si>
+  <si>
+    <t>pentode, 25W</t>
+  </si>
+  <si>
+    <t>LXH387USBD-150</t>
+  </si>
+  <si>
+    <t>6883</t>
+  </si>
+  <si>
+    <t>NYS367-2</t>
+  </si>
+  <si>
+    <t>NYS367-0</t>
+  </si>
+  <si>
+    <t>4304.6090</t>
+  </si>
+  <si>
+    <t>745</t>
+  </si>
+  <si>
+    <t>22k 2W</t>
+  </si>
+  <si>
+    <t>33k 2W</t>
+  </si>
+  <si>
+    <t>39k 2W</t>
+  </si>
+  <si>
+    <t>279-RR02J33KTB</t>
+  </si>
+  <si>
+    <t>279-RR02J39KTB</t>
   </si>
 </sst>
 </file>
@@ -1229,9 +1312,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1586,12 +1670,2275 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC11A494-757A-AD4A-AA7D-13F0C2E663D3}">
+  <dimension ref="A1:M68"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="G54" sqref="G54"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="25.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>165</v>
+      </c>
+      <c r="D7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" t="s">
+        <v>200</v>
+      </c>
+      <c r="F7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" t="s">
+        <v>199</v>
+      </c>
+      <c r="I7" t="str">
+        <f>IF(H7="","",RIGHT(H7,LEN(H7)-FIND("-",H7)))</f>
+        <v>R463I315040H2M</v>
+      </c>
+      <c r="J7">
+        <f>B7</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" t="s">
+        <v>144</v>
+      </c>
+      <c r="E8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" t="s">
+        <v>145</v>
+      </c>
+      <c r="H8" t="s">
+        <v>127</v>
+      </c>
+      <c r="I8" t="str">
+        <f t="shared" ref="I8:I55" si="0">IF(H8="","",RIGHT(H8,LEN(H8)-FIND("-",H8)))</f>
+        <v>EST477M100AN5AA</v>
+      </c>
+      <c r="J8">
+        <f t="shared" ref="J8:J55" si="1">B8</f>
+        <v>2</v>
+      </c>
+      <c r="L8" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" t="s">
+        <v>144</v>
+      </c>
+      <c r="E9" t="s">
+        <v>146</v>
+      </c>
+      <c r="F9" t="s">
+        <v>145</v>
+      </c>
+      <c r="H9" t="s">
+        <v>128</v>
+      </c>
+      <c r="I9" t="str">
+        <f t="shared" si="0"/>
+        <v>228CKS025M</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="L9" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>147</v>
+      </c>
+      <c r="B10">
+        <v>4</v>
+      </c>
+      <c r="C10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" t="s">
+        <v>144</v>
+      </c>
+      <c r="E10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" t="s">
+        <v>145</v>
+      </c>
+      <c r="H10" t="s">
+        <v>129</v>
+      </c>
+      <c r="I10" t="str">
+        <f t="shared" si="0"/>
+        <v>EEU-EE2W470S</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>148</v>
+      </c>
+      <c r="B11">
+        <v>6</v>
+      </c>
+      <c r="C11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" t="s">
+        <v>144</v>
+      </c>
+      <c r="E11" t="s">
+        <v>146</v>
+      </c>
+      <c r="F11" t="s">
+        <v>145</v>
+      </c>
+      <c r="H11" t="s">
+        <v>131</v>
+      </c>
+      <c r="I11" t="str">
+        <f t="shared" si="0"/>
+        <v>UPS2C470MHD1TO</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="L11" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>149</v>
+      </c>
+      <c r="B12">
+        <v>3</v>
+      </c>
+      <c r="C12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" t="s">
+        <v>144</v>
+      </c>
+      <c r="E12" t="s">
+        <v>150</v>
+      </c>
+      <c r="F12" t="s">
+        <v>145</v>
+      </c>
+      <c r="H12" t="s">
+        <v>134</v>
+      </c>
+      <c r="I12" t="str">
+        <f t="shared" si="0"/>
+        <v>UVR1E470MDD1TD</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="L12" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" t="s">
+        <v>144</v>
+      </c>
+      <c r="E13" t="s">
+        <v>20</v>
+      </c>
+      <c r="F13" t="s">
+        <v>145</v>
+      </c>
+      <c r="H13" t="s">
+        <v>130</v>
+      </c>
+      <c r="I13" t="str">
+        <f t="shared" si="0"/>
+        <v>UPM2W100MHD</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="L13" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" t="s">
+        <v>144</v>
+      </c>
+      <c r="E14" t="s">
+        <v>28</v>
+      </c>
+      <c r="F14" t="s">
+        <v>145</v>
+      </c>
+      <c r="H14" t="s">
+        <v>132</v>
+      </c>
+      <c r="I14" t="str">
+        <f t="shared" si="0"/>
+        <v>517D106M160CC6AE3</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" t="s">
+        <v>144</v>
+      </c>
+      <c r="E15" t="s">
+        <v>28</v>
+      </c>
+      <c r="F15" t="s">
+        <v>145</v>
+      </c>
+      <c r="H15" t="s">
+        <v>133</v>
+      </c>
+      <c r="I15" t="str">
+        <f t="shared" si="0"/>
+        <v>ECA-2DM100B</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16">
+        <v>4</v>
+      </c>
+      <c r="C16" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" t="s">
+        <v>151</v>
+      </c>
+      <c r="F16" t="s">
+        <v>14</v>
+      </c>
+      <c r="H16" t="s">
+        <v>135</v>
+      </c>
+      <c r="I16" t="str">
+        <f t="shared" si="0"/>
+        <v>MKP10-.226305P22</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="K16" t="s">
+        <v>225</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="M16" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17">
+        <v>4</v>
+      </c>
+      <c r="C17" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17" t="s">
+        <v>35</v>
+      </c>
+      <c r="E17" t="s">
+        <v>36</v>
+      </c>
+      <c r="F17" t="s">
+        <v>37</v>
+      </c>
+      <c r="H17" t="s">
+        <v>136</v>
+      </c>
+      <c r="I17" t="str">
+        <f t="shared" si="0"/>
+        <v>SF51-B</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="L17" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18">
+        <v>8</v>
+      </c>
+      <c r="C18" t="s">
+        <v>39</v>
+      </c>
+      <c r="D18" t="s">
+        <v>35</v>
+      </c>
+      <c r="E18" t="s">
+        <v>40</v>
+      </c>
+      <c r="F18" t="s">
+        <v>37</v>
+      </c>
+      <c r="H18" t="s">
+        <v>137</v>
+      </c>
+      <c r="I18" t="str">
+        <f t="shared" si="0"/>
+        <v>UF4007</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>41</v>
+      </c>
+      <c r="B19">
+        <v>6</v>
+      </c>
+      <c r="C19" t="s">
+        <v>42</v>
+      </c>
+      <c r="D19" t="s">
+        <v>43</v>
+      </c>
+      <c r="E19" t="s">
+        <v>152</v>
+      </c>
+      <c r="F19" t="s">
+        <v>44</v>
+      </c>
+      <c r="H19" t="s">
+        <v>138</v>
+      </c>
+      <c r="I19" t="str">
+        <f t="shared" si="0"/>
+        <v>BZX79C10</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>45</v>
+      </c>
+      <c r="B20">
+        <v>4</v>
+      </c>
+      <c r="C20" t="s">
+        <v>46</v>
+      </c>
+      <c r="D20" t="s">
+        <v>47</v>
+      </c>
+      <c r="E20" t="s">
+        <v>48</v>
+      </c>
+      <c r="F20" t="s">
+        <v>49</v>
+      </c>
+      <c r="H20" t="s">
+        <v>201</v>
+      </c>
+      <c r="I20" t="str">
+        <f t="shared" si="0"/>
+        <v>151033RS03000</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>50</v>
+      </c>
+      <c r="B21">
+        <v>2</v>
+      </c>
+      <c r="C21" t="s">
+        <v>51</v>
+      </c>
+      <c r="D21" t="s">
+        <v>52</v>
+      </c>
+      <c r="E21" t="s">
+        <v>166</v>
+      </c>
+      <c r="F21" t="s">
+        <v>52</v>
+      </c>
+      <c r="H21" t="s">
+        <v>176</v>
+      </c>
+      <c r="I21" t="str">
+        <f t="shared" si="0"/>
+        <v>HSE-B20250-040H</v>
+      </c>
+      <c r="J21">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>53</v>
+      </c>
+      <c r="B22">
+        <v>10</v>
+      </c>
+      <c r="C22" t="s">
+        <v>54</v>
+      </c>
+      <c r="D22" t="s">
+        <v>54</v>
+      </c>
+      <c r="E22" t="s">
+        <v>55</v>
+      </c>
+      <c r="F22" t="s">
+        <v>56</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="I22" t="str">
+        <f t="shared" si="0"/>
+        <v>5441537</v>
+      </c>
+      <c r="J22">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="M22" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>57</v>
+      </c>
+      <c r="B23">
+        <v>2</v>
+      </c>
+      <c r="C23" t="s">
+        <v>58</v>
+      </c>
+      <c r="D23" t="s">
+        <v>58</v>
+      </c>
+      <c r="E23" t="s">
+        <v>167</v>
+      </c>
+      <c r="F23" t="s">
+        <v>59</v>
+      </c>
+      <c r="H23" t="s">
+        <v>218</v>
+      </c>
+      <c r="I23" t="str">
+        <f t="shared" si="0"/>
+        <v>282838-6</v>
+      </c>
+      <c r="J23">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="M23" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>60</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24" t="s">
+        <v>61</v>
+      </c>
+      <c r="D24" t="s">
+        <v>62</v>
+      </c>
+      <c r="E24" t="s">
+        <v>63</v>
+      </c>
+      <c r="F24" t="s">
+        <v>64</v>
+      </c>
+      <c r="H24" t="s">
+        <v>173</v>
+      </c>
+      <c r="I24" t="str">
+        <f t="shared" si="0"/>
+        <v>FQPF8N60C</v>
+      </c>
+      <c r="J24">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>65</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25" t="s">
+        <v>66</v>
+      </c>
+      <c r="D25" t="s">
+        <v>67</v>
+      </c>
+      <c r="E25" t="s">
+        <v>63</v>
+      </c>
+      <c r="F25" t="s">
+        <v>68</v>
+      </c>
+      <c r="H25" t="s">
+        <v>172</v>
+      </c>
+      <c r="I25" t="str">
+        <f t="shared" si="0"/>
+        <v>FQPF7P20</v>
+      </c>
+      <c r="J25">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>69</v>
+      </c>
+      <c r="B26">
+        <v>12</v>
+      </c>
+      <c r="C26" t="s">
+        <v>70</v>
+      </c>
+      <c r="D26" t="s">
+        <v>71</v>
+      </c>
+      <c r="E26" t="s">
+        <v>72</v>
+      </c>
+      <c r="F26" t="s">
+        <v>73</v>
+      </c>
+      <c r="H26" t="s">
+        <v>171</v>
+      </c>
+      <c r="I26" t="str">
+        <f t="shared" si="0"/>
+        <v>2N5551</v>
+      </c>
+      <c r="J26">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>74</v>
+      </c>
+      <c r="B27">
+        <v>4</v>
+      </c>
+      <c r="C27" t="s">
+        <v>75</v>
+      </c>
+      <c r="D27" t="s">
+        <v>62</v>
+      </c>
+      <c r="E27" t="s">
+        <v>76</v>
+      </c>
+      <c r="F27" t="s">
+        <v>64</v>
+      </c>
+      <c r="H27" t="s">
+        <v>170</v>
+      </c>
+      <c r="I27" t="str">
+        <f t="shared" si="0"/>
+        <v>STU9HN65M2</v>
+      </c>
+      <c r="J27">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>77</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28" t="s">
+        <v>78</v>
+      </c>
+      <c r="D28" t="s">
+        <v>79</v>
+      </c>
+      <c r="E28" t="s">
+        <v>153</v>
+      </c>
+      <c r="F28" t="s">
+        <v>80</v>
+      </c>
+      <c r="H28" t="s">
+        <v>139</v>
+      </c>
+      <c r="I28" t="str">
+        <f t="shared" si="0"/>
+        <v>RS00510R00FE73</v>
+      </c>
+      <c r="J28">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>240</v>
+      </c>
+      <c r="B29">
+        <v>10</v>
+      </c>
+      <c r="C29" t="s">
+        <v>81</v>
+      </c>
+      <c r="D29" t="s">
+        <v>79</v>
+      </c>
+      <c r="E29" t="s">
+        <v>82</v>
+      </c>
+      <c r="F29" t="s">
+        <v>80</v>
+      </c>
+      <c r="H29" t="s">
+        <v>182</v>
+      </c>
+      <c r="I29" t="str">
+        <f t="shared" si="0"/>
+        <v>MF0207FRE52-100R</v>
+      </c>
+      <c r="J29">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>237</v>
+      </c>
+      <c r="B30">
+        <v>4</v>
+      </c>
+      <c r="C30" t="s">
+        <v>83</v>
+      </c>
+      <c r="D30" t="s">
+        <v>79</v>
+      </c>
+      <c r="E30" t="s">
+        <v>82</v>
+      </c>
+      <c r="F30" t="s">
+        <v>80</v>
+      </c>
+      <c r="H30" t="s">
+        <v>183</v>
+      </c>
+      <c r="I30" t="str">
+        <f t="shared" si="0"/>
+        <v>MF0207FTE52-22K</v>
+      </c>
+      <c r="J30">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>238</v>
+      </c>
+      <c r="B31">
+        <v>6</v>
+      </c>
+      <c r="C31" t="s">
+        <v>84</v>
+      </c>
+      <c r="D31" t="s">
+        <v>79</v>
+      </c>
+      <c r="E31" t="s">
+        <v>82</v>
+      </c>
+      <c r="F31" t="s">
+        <v>80</v>
+      </c>
+      <c r="H31" t="s">
+        <v>184</v>
+      </c>
+      <c r="I31" t="str">
+        <f t="shared" si="0"/>
+        <v>MF0207FRE52-1M</v>
+      </c>
+      <c r="J31">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>239</v>
+      </c>
+      <c r="B32">
+        <v>3</v>
+      </c>
+      <c r="C32" t="s">
+        <v>85</v>
+      </c>
+      <c r="D32" t="s">
+        <v>79</v>
+      </c>
+      <c r="E32" t="s">
+        <v>82</v>
+      </c>
+      <c r="F32" t="s">
+        <v>80</v>
+      </c>
+      <c r="H32" t="s">
+        <v>185</v>
+      </c>
+      <c r="I32" t="str">
+        <f t="shared" si="0"/>
+        <v>LR1F330K</v>
+      </c>
+      <c r="J32">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>241</v>
+      </c>
+      <c r="B33">
+        <v>1</v>
+      </c>
+      <c r="C33" t="s">
+        <v>87</v>
+      </c>
+      <c r="D33" t="s">
+        <v>79</v>
+      </c>
+      <c r="E33" t="s">
+        <v>82</v>
+      </c>
+      <c r="F33" t="s">
+        <v>80</v>
+      </c>
+      <c r="H33" t="s">
+        <v>186</v>
+      </c>
+      <c r="I33" t="str">
+        <f t="shared" si="0"/>
+        <v>LR1F22R</v>
+      </c>
+      <c r="J33">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>242</v>
+      </c>
+      <c r="B34">
+        <v>1</v>
+      </c>
+      <c r="C34" t="s">
+        <v>88</v>
+      </c>
+      <c r="D34" t="s">
+        <v>79</v>
+      </c>
+      <c r="E34" t="s">
+        <v>82</v>
+      </c>
+      <c r="F34" t="s">
+        <v>80</v>
+      </c>
+      <c r="H34" t="s">
+        <v>187</v>
+      </c>
+      <c r="I34" t="str">
+        <f t="shared" si="0"/>
+        <v>LR1F10R</v>
+      </c>
+      <c r="J34">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>243</v>
+      </c>
+      <c r="B35">
+        <v>3</v>
+      </c>
+      <c r="C35" t="s">
+        <v>89</v>
+      </c>
+      <c r="D35" t="s">
+        <v>79</v>
+      </c>
+      <c r="E35" t="s">
+        <v>82</v>
+      </c>
+      <c r="F35" t="s">
+        <v>80</v>
+      </c>
+      <c r="H35" t="s">
+        <v>188</v>
+      </c>
+      <c r="I35" t="str">
+        <f t="shared" si="0"/>
+        <v>MF0207FRE52-47K</v>
+      </c>
+      <c r="J35">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>90</v>
+      </c>
+      <c r="B36">
+        <v>2</v>
+      </c>
+      <c r="C36" t="s">
+        <v>91</v>
+      </c>
+      <c r="D36" t="s">
+        <v>79</v>
+      </c>
+      <c r="E36" t="s">
+        <v>82</v>
+      </c>
+      <c r="F36" t="s">
+        <v>80</v>
+      </c>
+      <c r="H36" t="s">
+        <v>189</v>
+      </c>
+      <c r="I36" t="str">
+        <f t="shared" si="0"/>
+        <v>LR1F680R</v>
+      </c>
+      <c r="J36">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>92</v>
+      </c>
+      <c r="B37">
+        <v>2</v>
+      </c>
+      <c r="C37" t="s">
+        <v>93</v>
+      </c>
+      <c r="D37" t="s">
+        <v>79</v>
+      </c>
+      <c r="E37" t="s">
+        <v>82</v>
+      </c>
+      <c r="F37" t="s">
+        <v>80</v>
+      </c>
+      <c r="H37" t="s">
+        <v>190</v>
+      </c>
+      <c r="I37" t="str">
+        <f t="shared" si="0"/>
+        <v>LR1F100K</v>
+      </c>
+      <c r="J37">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>94</v>
+      </c>
+      <c r="B38">
+        <v>2</v>
+      </c>
+      <c r="C38" t="s">
+        <v>95</v>
+      </c>
+      <c r="D38" t="s">
+        <v>79</v>
+      </c>
+      <c r="E38" t="s">
+        <v>82</v>
+      </c>
+      <c r="F38" t="s">
+        <v>80</v>
+      </c>
+      <c r="H38" t="s">
+        <v>191</v>
+      </c>
+      <c r="I38" t="str">
+        <f t="shared" si="0"/>
+        <v>LR1F470R</v>
+      </c>
+      <c r="J38">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>96</v>
+      </c>
+      <c r="B39">
+        <v>12</v>
+      </c>
+      <c r="C39" t="s">
+        <v>97</v>
+      </c>
+      <c r="D39" t="s">
+        <v>79</v>
+      </c>
+      <c r="E39" t="s">
+        <v>82</v>
+      </c>
+      <c r="F39" t="s">
+        <v>80</v>
+      </c>
+      <c r="H39" t="s">
+        <v>192</v>
+      </c>
+      <c r="I39" t="str">
+        <f t="shared" si="0"/>
+        <v>MBB02070C1001FRP</v>
+      </c>
+      <c r="J39">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>98</v>
+      </c>
+      <c r="B40">
+        <v>4</v>
+      </c>
+      <c r="C40" t="s">
+        <v>99</v>
+      </c>
+      <c r="D40" t="s">
+        <v>79</v>
+      </c>
+      <c r="E40" t="s">
+        <v>100</v>
+      </c>
+      <c r="F40" t="s">
+        <v>80</v>
+      </c>
+      <c r="H40" t="s">
+        <v>196</v>
+      </c>
+      <c r="I40" t="str">
+        <f t="shared" si="0"/>
+        <v>FMF200FTE52-220K</v>
+      </c>
+      <c r="J40">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>101</v>
+      </c>
+      <c r="B41">
+        <v>4</v>
+      </c>
+      <c r="C41" t="s">
+        <v>102</v>
+      </c>
+      <c r="D41" t="s">
+        <v>79</v>
+      </c>
+      <c r="E41" t="s">
+        <v>82</v>
+      </c>
+      <c r="F41" t="s">
+        <v>80</v>
+      </c>
+      <c r="H41" t="s">
+        <v>193</v>
+      </c>
+      <c r="I41" t="str">
+        <f t="shared" si="0"/>
+        <v>LR1F220K</v>
+      </c>
+      <c r="J41">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>103</v>
+      </c>
+      <c r="B42">
+        <v>4</v>
+      </c>
+      <c r="C42" t="s">
+        <v>104</v>
+      </c>
+      <c r="D42" t="s">
+        <v>79</v>
+      </c>
+      <c r="E42" t="s">
+        <v>82</v>
+      </c>
+      <c r="F42" t="s">
+        <v>80</v>
+      </c>
+      <c r="H42" t="s">
+        <v>194</v>
+      </c>
+      <c r="I42" t="str">
+        <f t="shared" si="0"/>
+        <v>LR1F390R</v>
+      </c>
+      <c r="J42">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>105</v>
+      </c>
+      <c r="B43">
+        <v>2</v>
+      </c>
+      <c r="C43" t="s">
+        <v>260</v>
+      </c>
+      <c r="D43" t="s">
+        <v>79</v>
+      </c>
+      <c r="E43" t="s">
+        <v>100</v>
+      </c>
+      <c r="F43" t="s">
+        <v>80</v>
+      </c>
+      <c r="H43" t="s">
+        <v>216</v>
+      </c>
+      <c r="I43" t="str">
+        <f t="shared" si="0"/>
+        <v>RR02J22KTB</v>
+      </c>
+      <c r="J43">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>105</v>
+      </c>
+      <c r="B44">
+        <v>2</v>
+      </c>
+      <c r="C44" t="s">
+        <v>261</v>
+      </c>
+      <c r="D44" t="s">
+        <v>79</v>
+      </c>
+      <c r="E44" t="s">
+        <v>100</v>
+      </c>
+      <c r="F44" t="s">
+        <v>80</v>
+      </c>
+      <c r="H44" t="s">
+        <v>263</v>
+      </c>
+      <c r="I44" t="str">
+        <f t="shared" ref="I44" si="2">IF(H44="","",RIGHT(H44,LEN(H44)-FIND("-",H44)))</f>
+        <v>RR02J33KTB</v>
+      </c>
+      <c r="J44">
+        <f t="shared" ref="J44" si="3">B44</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>105</v>
+      </c>
+      <c r="B45">
+        <v>2</v>
+      </c>
+      <c r="C45" t="s">
+        <v>262</v>
+      </c>
+      <c r="D45" t="s">
+        <v>79</v>
+      </c>
+      <c r="E45" t="s">
+        <v>100</v>
+      </c>
+      <c r="F45" t="s">
+        <v>80</v>
+      </c>
+      <c r="H45" t="s">
+        <v>264</v>
+      </c>
+      <c r="I45" t="str">
+        <f t="shared" ref="I45" si="4">IF(H45="","",RIGHT(H45,LEN(H45)-FIND("-",H45)))</f>
+        <v>RR02J39KTB</v>
+      </c>
+      <c r="J45">
+        <f t="shared" ref="J45" si="5">B45</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>106</v>
+      </c>
+      <c r="B46">
+        <v>4</v>
+      </c>
+      <c r="C46" t="s">
+        <v>107</v>
+      </c>
+      <c r="D46" t="s">
+        <v>79</v>
+      </c>
+      <c r="E46" t="s">
+        <v>100</v>
+      </c>
+      <c r="F46" t="s">
+        <v>80</v>
+      </c>
+      <c r="H46" t="s">
+        <v>197</v>
+      </c>
+      <c r="I46" t="str">
+        <f t="shared" si="0"/>
+        <v>5083NW47K00JA100</v>
+      </c>
+      <c r="J46">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>108</v>
+      </c>
+      <c r="B47">
+        <v>4</v>
+      </c>
+      <c r="C47" t="s">
+        <v>109</v>
+      </c>
+      <c r="D47" t="s">
+        <v>79</v>
+      </c>
+      <c r="E47" t="s">
+        <v>82</v>
+      </c>
+      <c r="F47" t="s">
+        <v>80</v>
+      </c>
+      <c r="H47" t="s">
+        <v>187</v>
+      </c>
+      <c r="I47" t="str">
+        <f t="shared" si="0"/>
+        <v>LR1F10R</v>
+      </c>
+      <c r="J47">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>110</v>
+      </c>
+      <c r="B48">
+        <v>4</v>
+      </c>
+      <c r="C48" t="s">
+        <v>111</v>
+      </c>
+      <c r="D48" t="s">
+        <v>79</v>
+      </c>
+      <c r="E48" t="s">
+        <v>100</v>
+      </c>
+      <c r="F48" t="s">
+        <v>80</v>
+      </c>
+      <c r="H48" t="s">
+        <v>198</v>
+      </c>
+      <c r="I48" t="str">
+        <f t="shared" si="0"/>
+        <v>5083NW1K000J</v>
+      </c>
+      <c r="J48">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>112</v>
+      </c>
+      <c r="B49">
+        <v>4</v>
+      </c>
+      <c r="C49" t="s">
+        <v>113</v>
+      </c>
+      <c r="D49" t="s">
+        <v>79</v>
+      </c>
+      <c r="E49" t="s">
+        <v>82</v>
+      </c>
+      <c r="F49" t="s">
+        <v>80</v>
+      </c>
+      <c r="H49" t="s">
+        <v>195</v>
+      </c>
+      <c r="I49" t="str">
+        <f t="shared" si="0"/>
+        <v>LR1F270R</v>
+      </c>
+      <c r="J49">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>114</v>
+      </c>
+      <c r="B50">
+        <v>2</v>
+      </c>
+      <c r="C50" t="s">
+        <v>141</v>
+      </c>
+      <c r="D50" t="s">
+        <v>79</v>
+      </c>
+      <c r="E50" t="s">
+        <v>100</v>
+      </c>
+      <c r="F50" t="s">
+        <v>80</v>
+      </c>
+      <c r="H50" t="s">
+        <v>140</v>
+      </c>
+      <c r="I50" t="str">
+        <f t="shared" si="0"/>
+        <v>G00310R00FE7080</v>
+      </c>
+      <c r="J50">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>245</v>
+      </c>
+      <c r="B51">
+        <v>5</v>
+      </c>
+      <c r="C51" t="s">
+        <v>117</v>
+      </c>
+      <c r="D51" t="s">
+        <v>161</v>
+      </c>
+      <c r="E51" t="s">
+        <v>116</v>
+      </c>
+      <c r="F51" t="s">
+        <v>162</v>
+      </c>
+      <c r="H51" t="s">
+        <v>177</v>
+      </c>
+      <c r="I51" t="str">
+        <f t="shared" si="0"/>
+        <v>3339P-1-503LF</v>
+      </c>
+      <c r="J51">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>244</v>
+      </c>
+      <c r="B52">
+        <v>3</v>
+      </c>
+      <c r="C52" t="s">
+        <v>95</v>
+      </c>
+      <c r="D52" t="s">
+        <v>161</v>
+      </c>
+      <c r="E52" t="s">
+        <v>116</v>
+      </c>
+      <c r="F52" t="s">
+        <v>162</v>
+      </c>
+      <c r="H52" t="s">
+        <v>178</v>
+      </c>
+      <c r="I52" t="str">
+        <f t="shared" si="0"/>
+        <v>3339P-1-501LF</v>
+      </c>
+      <c r="J52">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>115</v>
+      </c>
+      <c r="B53">
+        <v>2</v>
+      </c>
+      <c r="C53" t="s">
+        <v>97</v>
+      </c>
+      <c r="D53" t="s">
+        <v>161</v>
+      </c>
+      <c r="E53" t="s">
+        <v>116</v>
+      </c>
+      <c r="F53" t="s">
+        <v>162</v>
+      </c>
+      <c r="H53" t="s">
+        <v>179</v>
+      </c>
+      <c r="I53" t="str">
+        <f t="shared" si="0"/>
+        <v>3339P-1-102LF</v>
+      </c>
+      <c r="J53">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>118</v>
+      </c>
+      <c r="B54">
+        <v>1</v>
+      </c>
+      <c r="C54" t="s">
+        <v>119</v>
+      </c>
+      <c r="D54" t="s">
+        <v>120</v>
+      </c>
+      <c r="E54" t="s">
+        <v>121</v>
+      </c>
+      <c r="F54" t="s">
+        <v>122</v>
+      </c>
+      <c r="H54" t="s">
+        <v>180</v>
+      </c>
+      <c r="I54" t="str">
+        <f t="shared" si="0"/>
+        <v>CL140</v>
+      </c>
+      <c r="J54">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>123</v>
+      </c>
+      <c r="B55">
+        <v>10</v>
+      </c>
+      <c r="C55" t="s">
+        <v>124</v>
+      </c>
+      <c r="D55" t="s">
+        <v>124</v>
+      </c>
+      <c r="E55" t="s">
+        <v>125</v>
+      </c>
+      <c r="F55" t="s">
+        <v>126</v>
+      </c>
+      <c r="H55" t="s">
+        <v>181</v>
+      </c>
+      <c r="I55" t="str">
+        <f t="shared" si="0"/>
+        <v>5006</v>
+      </c>
+      <c r="J55">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A59" s="2" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>246</v>
+      </c>
+      <c r="B60">
+        <v>2</v>
+      </c>
+      <c r="C60" t="s">
+        <v>247</v>
+      </c>
+      <c r="D60" t="s">
+        <v>247</v>
+      </c>
+      <c r="E60" t="s">
+        <v>248</v>
+      </c>
+      <c r="F60" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>250</v>
+      </c>
+      <c r="B61">
+        <v>4</v>
+      </c>
+      <c r="C61" t="s">
+        <v>251</v>
+      </c>
+      <c r="D61" t="s">
+        <v>251</v>
+      </c>
+      <c r="E61" t="s">
+        <v>252</v>
+      </c>
+      <c r="F61" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>203</v>
+      </c>
+      <c r="B62">
+        <v>1</v>
+      </c>
+      <c r="H62" t="s">
+        <v>212</v>
+      </c>
+      <c r="I62" t="s">
+        <v>254</v>
+      </c>
+      <c r="J62">
+        <v>1</v>
+      </c>
+      <c r="M62" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>204</v>
+      </c>
+      <c r="B63">
+        <v>2</v>
+      </c>
+      <c r="H63" t="s">
+        <v>205</v>
+      </c>
+      <c r="I63" t="s">
+        <v>255</v>
+      </c>
+      <c r="J63">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>206</v>
+      </c>
+      <c r="B64">
+        <v>1</v>
+      </c>
+      <c r="H64" t="s">
+        <v>207</v>
+      </c>
+      <c r="I64" t="s">
+        <v>256</v>
+      </c>
+      <c r="J64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>208</v>
+      </c>
+      <c r="B65">
+        <v>1</v>
+      </c>
+      <c r="H65" t="s">
+        <v>209</v>
+      </c>
+      <c r="I65" t="s">
+        <v>257</v>
+      </c>
+      <c r="J65">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>210</v>
+      </c>
+      <c r="B66">
+        <v>1</v>
+      </c>
+      <c r="H66" t="s">
+        <v>211</v>
+      </c>
+      <c r="I66" t="s">
+        <v>258</v>
+      </c>
+      <c r="J66">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>213</v>
+      </c>
+      <c r="B67">
+        <v>4</v>
+      </c>
+      <c r="H67" t="s">
+        <v>214</v>
+      </c>
+      <c r="I67" t="s">
+        <v>259</v>
+      </c>
+      <c r="J67">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>215</v>
+      </c>
+      <c r="M68" t="s">
+        <v>221</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34311C58-04AE-2548-B3A2-A4F7A63B9371}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B270E01A-C831-5B46-99F7-CEE7B1F93A2B}">
+  <dimension ref="A1:B54"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>222</v>
+      </c>
+      <c r="B1" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>199</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>128</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>129</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>131</v>
+      </c>
+      <c r="B6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>134</v>
+      </c>
+      <c r="B7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>130</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>132</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>133</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>135</v>
+      </c>
+      <c r="B11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>136</v>
+      </c>
+      <c r="B12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>137</v>
+      </c>
+      <c r="B13">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>138</v>
+      </c>
+      <c r="B14">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>201</v>
+      </c>
+      <c r="B15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>176</v>
+      </c>
+      <c r="B16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>174</v>
+      </c>
+      <c r="B17">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>218</v>
+      </c>
+      <c r="B18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>173</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>172</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>171</v>
+      </c>
+      <c r="B21">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>170</v>
+      </c>
+      <c r="B22">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>139</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>182</v>
+      </c>
+      <c r="B24">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>183</v>
+      </c>
+      <c r="B25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>184</v>
+      </c>
+      <c r="B26">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>185</v>
+      </c>
+      <c r="B27">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>186</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>187</v>
+      </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>188</v>
+      </c>
+      <c r="B30">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>189</v>
+      </c>
+      <c r="B31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>190</v>
+      </c>
+      <c r="B32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>191</v>
+      </c>
+      <c r="B33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>192</v>
+      </c>
+      <c r="B34">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>196</v>
+      </c>
+      <c r="B35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>193</v>
+      </c>
+      <c r="B36">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>194</v>
+      </c>
+      <c r="B37">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>216</v>
+      </c>
+      <c r="B38">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>197</v>
+      </c>
+      <c r="B39">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>187</v>
+      </c>
+      <c r="B40">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>198</v>
+      </c>
+      <c r="B41">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>195</v>
+      </c>
+      <c r="B42">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>140</v>
+      </c>
+      <c r="B43">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>177</v>
+      </c>
+      <c r="B44">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>178</v>
+      </c>
+      <c r="B45">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>179</v>
+      </c>
+      <c r="B46">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>180</v>
+      </c>
+      <c r="B47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>181</v>
+      </c>
+      <c r="B48">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>212</v>
+      </c>
+      <c r="B49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>205</v>
+      </c>
+      <c r="B50">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>207</v>
+      </c>
+      <c r="B51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>209</v>
+      </c>
+      <c r="B52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>211</v>
+      </c>
+      <c r="B53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>214</v>
+      </c>
+      <c r="B54">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB340298-E73E-9A41-B0B6-F93061A8A872}">
-  <dimension ref="A1:N66"/>
+  <dimension ref="A1:N65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="K52" sqref="K52"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1609,7 +3956,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
@@ -1617,7 +3964,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
@@ -1625,7 +3972,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
@@ -1633,7 +3980,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
@@ -1667,22 +4014,22 @@
         <v>11</v>
       </c>
       <c r="H6" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="J6" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="K6" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="L6" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="M6" t="s">
+        <v>227</v>
+      </c>
+      <c r="N6" t="s">
         <v>229</v>
-      </c>
-      <c r="N6" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
@@ -1693,19 +4040,19 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D7" t="s">
         <v>13</v>
       </c>
       <c r="E7" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="F7" t="s">
         <v>14</v>
       </c>
       <c r="H7" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="J7" t="str">
         <f>IF(H7="","",RIGHT(H7,LEN(H7)-FIND("-",H7)))</f>
@@ -1727,27 +4074,27 @@
         <v>16</v>
       </c>
       <c r="D8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E8" t="s">
         <v>17</v>
       </c>
       <c r="F8" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J8" t="str">
-        <f t="shared" ref="J8:J65" si="0">IF(H8="","",RIGHT(H8,LEN(H8)-FIND("-",H8)))</f>
+        <f t="shared" ref="J8:J64" si="0">IF(H8="","",RIGHT(H8,LEN(H8)-FIND("-",H8)))</f>
         <v>EST477M100AN5AA</v>
       </c>
       <c r="K8">
-        <f t="shared" ref="K8:K65" si="1">B8</f>
+        <f t="shared" ref="K8:K64" si="1">B8</f>
         <v>2</v>
       </c>
       <c r="M8" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
@@ -1761,16 +4108,16 @@
         <v>19</v>
       </c>
       <c r="D9" t="s">
+        <v>144</v>
+      </c>
+      <c r="E9" t="s">
+        <v>146</v>
+      </c>
+      <c r="F9" t="s">
         <v>145</v>
       </c>
-      <c r="E9" t="s">
-        <v>147</v>
-      </c>
-      <c r="F9" t="s">
-        <v>146</v>
-      </c>
       <c r="H9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J9" t="str">
         <f t="shared" si="0"/>
@@ -1781,12 +4128,12 @@
         <v>2</v>
       </c>
       <c r="M9" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B10">
         <v>4</v>
@@ -1795,16 +4142,16 @@
         <v>21</v>
       </c>
       <c r="D10" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E10" t="s">
         <v>17</v>
       </c>
       <c r="F10" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J10" t="str">
         <f t="shared" si="0"/>
@@ -1817,7 +4164,7 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B11">
         <v>6</v>
@@ -1826,16 +4173,16 @@
         <v>22</v>
       </c>
       <c r="D11" t="s">
+        <v>144</v>
+      </c>
+      <c r="E11" t="s">
+        <v>146</v>
+      </c>
+      <c r="F11" t="s">
         <v>145</v>
       </c>
-      <c r="E11" t="s">
-        <v>147</v>
-      </c>
-      <c r="F11" t="s">
-        <v>146</v>
-      </c>
       <c r="H11" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="J11" t="str">
         <f t="shared" si="0"/>
@@ -1846,12 +4193,12 @@
         <v>6</v>
       </c>
       <c r="M11" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B12">
         <v>3</v>
@@ -1860,16 +4207,16 @@
         <v>23</v>
       </c>
       <c r="D12" t="s">
+        <v>144</v>
+      </c>
+      <c r="E12" t="s">
+        <v>150</v>
+      </c>
+      <c r="F12" t="s">
         <v>145</v>
       </c>
-      <c r="E12" t="s">
-        <v>151</v>
-      </c>
-      <c r="F12" t="s">
-        <v>146</v>
-      </c>
       <c r="H12" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J12" t="str">
         <f t="shared" si="0"/>
@@ -1880,7 +4227,7 @@
         <v>3</v>
       </c>
       <c r="M12" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
@@ -1894,16 +4241,16 @@
         <v>25</v>
       </c>
       <c r="D13" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E13" t="s">
         <v>20</v>
       </c>
       <c r="F13" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H13" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="J13" t="str">
         <f t="shared" si="0"/>
@@ -1914,7 +4261,7 @@
         <v>1</v>
       </c>
       <c r="M13" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
@@ -1928,16 +4275,16 @@
         <v>27</v>
       </c>
       <c r="D14" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E14" t="s">
         <v>28</v>
       </c>
       <c r="F14" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J14" t="str">
         <f t="shared" si="0"/>
@@ -1959,16 +4306,16 @@
         <v>30</v>
       </c>
       <c r="D15" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E15" t="s">
         <v>28</v>
       </c>
       <c r="F15" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H15" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J15" t="str">
         <f t="shared" si="0"/>
@@ -1993,13 +4340,13 @@
         <v>13</v>
       </c>
       <c r="E16" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F16" t="s">
         <v>14</v>
       </c>
       <c r="H16" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J16" t="str">
         <f t="shared" si="0"/>
@@ -2010,13 +4357,13 @@
         <v>4</v>
       </c>
       <c r="L16" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M16" s="1" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="N16" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
@@ -2039,7 +4386,7 @@
         <v>37</v>
       </c>
       <c r="H17" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J17" t="str">
         <f t="shared" si="0"/>
@@ -2050,7 +4397,7 @@
         <v>4</v>
       </c>
       <c r="M17" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
@@ -2073,7 +4420,7 @@
         <v>37</v>
       </c>
       <c r="H18" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="J18" t="str">
         <f t="shared" si="0"/>
@@ -2098,13 +4445,13 @@
         <v>43</v>
       </c>
       <c r="E19" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F19" t="s">
         <v>44</v>
       </c>
       <c r="H19" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="J19" t="str">
         <f t="shared" si="0"/>
@@ -2135,7 +4482,7 @@
         <v>49</v>
       </c>
       <c r="H20" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="J20" t="str">
         <f t="shared" si="0"/>
@@ -2160,13 +4507,13 @@
         <v>52</v>
       </c>
       <c r="E21" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="F21" t="s">
         <v>52</v>
       </c>
       <c r="H21" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="J21" t="str">
         <f t="shared" si="0"/>
@@ -2197,10 +4544,10 @@
         <v>56</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="I22" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="J22" t="str">
         <f t="shared" si="0"/>
@@ -2225,16 +4572,16 @@
         <v>58</v>
       </c>
       <c r="E23" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="F23" t="s">
         <v>59</v>
       </c>
       <c r="H23" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="I23" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="J23" t="str">
         <f t="shared" si="0"/>
@@ -2265,7 +4612,7 @@
         <v>64</v>
       </c>
       <c r="H24" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="J24" t="str">
         <f t="shared" si="0"/>
@@ -2296,7 +4643,7 @@
         <v>68</v>
       </c>
       <c r="H25" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="J25" t="str">
         <f t="shared" si="0"/>
@@ -2327,7 +4674,7 @@
         <v>73</v>
       </c>
       <c r="H26" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J26" t="str">
         <f t="shared" si="0"/>
@@ -2358,7 +4705,7 @@
         <v>64</v>
       </c>
       <c r="H27" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="J27" t="str">
         <f t="shared" si="0"/>
@@ -2383,13 +4730,13 @@
         <v>79</v>
       </c>
       <c r="E28" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F28" t="s">
         <v>80</v>
       </c>
       <c r="H28" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="J28" t="str">
         <f t="shared" si="0"/>
@@ -2402,7 +4749,7 @@
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B29">
         <v>12</v>
@@ -2420,7 +4767,7 @@
         <v>80</v>
       </c>
       <c r="H29" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="J29" t="str">
         <f t="shared" si="0"/>
@@ -2433,13 +4780,13 @@
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B30">
         <v>4</v>
       </c>
       <c r="C30" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D30" t="s">
         <v>79</v>
@@ -2451,7 +4798,7 @@
         <v>80</v>
       </c>
       <c r="H30" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="J30" t="str">
         <f t="shared" si="0"/>
@@ -2464,13 +4811,13 @@
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B31">
         <v>6</v>
       </c>
       <c r="C31" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D31" t="s">
         <v>79</v>
@@ -2482,7 +4829,7 @@
         <v>80</v>
       </c>
       <c r="H31" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="J31" t="str">
         <f t="shared" si="0"/>
@@ -2495,13 +4842,13 @@
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B32">
         <v>3</v>
       </c>
       <c r="C32" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D32" t="s">
         <v>79</v>
@@ -2513,7 +4860,7 @@
         <v>80</v>
       </c>
       <c r="H32" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="J32" t="str">
         <f t="shared" si="0"/>
@@ -2526,13 +4873,13 @@
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B33">
         <v>1</v>
       </c>
       <c r="C33" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D33" t="s">
         <v>79</v>
@@ -2544,7 +4891,7 @@
         <v>80</v>
       </c>
       <c r="H33" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="J33" t="str">
         <f t="shared" si="0"/>
@@ -2557,13 +4904,13 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B34">
         <v>1</v>
       </c>
       <c r="C34" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D34" t="s">
         <v>79</v>
@@ -2575,7 +4922,7 @@
         <v>80</v>
       </c>
       <c r="H34" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="J34" t="str">
         <f t="shared" si="0"/>
@@ -2588,13 +4935,13 @@
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B35">
         <v>3</v>
       </c>
       <c r="C35" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D35" t="s">
         <v>79</v>
@@ -2606,7 +4953,7 @@
         <v>80</v>
       </c>
       <c r="H35" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="J35" t="str">
         <f t="shared" si="0"/>
@@ -2619,13 +4966,13 @@
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>161</v>
+        <v>90</v>
       </c>
       <c r="B36">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C36" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="D36" t="s">
         <v>79</v>
@@ -2636,24 +4983,27 @@
       <c r="F36" t="s">
         <v>80</v>
       </c>
+      <c r="H36" t="s">
+        <v>189</v>
+      </c>
       <c r="J36" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>LR1F680R</v>
       </c>
       <c r="K36">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B37">
         <v>2</v>
       </c>
       <c r="C37" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D37" t="s">
         <v>79</v>
@@ -2665,11 +5015,11 @@
         <v>80</v>
       </c>
       <c r="H37" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="J37" t="str">
         <f t="shared" si="0"/>
-        <v>LR1F680R</v>
+        <v>LR1F100K</v>
       </c>
       <c r="K37">
         <f t="shared" si="1"/>
@@ -2678,13 +5028,13 @@
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B38">
         <v>2</v>
       </c>
       <c r="C38" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D38" t="s">
         <v>79</v>
@@ -2696,11 +5046,11 @@
         <v>80</v>
       </c>
       <c r="H38" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="J38" t="str">
         <f t="shared" si="0"/>
-        <v>LR1F100K</v>
+        <v>LR1F470R</v>
       </c>
       <c r="K38">
         <f t="shared" si="1"/>
@@ -2709,13 +5059,13 @@
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B39">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="C39" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D39" t="s">
         <v>79</v>
@@ -2727,73 +5077,73 @@
         <v>80</v>
       </c>
       <c r="H39" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="J39" t="str">
         <f t="shared" si="0"/>
-        <v>LR1F470R</v>
+        <v>MBB02070C1001FRP</v>
       </c>
       <c r="K39">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B40">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C40" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D40" t="s">
         <v>79</v>
       </c>
       <c r="E40" t="s">
-        <v>82</v>
+        <v>100</v>
       </c>
       <c r="F40" t="s">
         <v>80</v>
       </c>
       <c r="H40" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="J40" t="str">
         <f t="shared" si="0"/>
-        <v>MBB02070C1001FRP</v>
+        <v>FMF200FTE52-220K</v>
       </c>
       <c r="K40">
         <f t="shared" si="1"/>
-        <v>12</v>
+        <v>4</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B41">
         <v>4</v>
       </c>
       <c r="C41" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="D41" t="s">
         <v>79</v>
       </c>
       <c r="E41" t="s">
-        <v>101</v>
+        <v>82</v>
       </c>
       <c r="F41" t="s">
         <v>80</v>
       </c>
       <c r="H41" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="J41" t="str">
         <f t="shared" si="0"/>
-        <v>FMF200FTE52-220K</v>
+        <v>LR1F220K</v>
       </c>
       <c r="K41">
         <f t="shared" si="1"/>
@@ -2802,13 +5152,13 @@
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B42">
         <v>4</v>
       </c>
       <c r="C42" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D42" t="s">
         <v>79</v>
@@ -2820,11 +5170,11 @@
         <v>80</v>
       </c>
       <c r="H42" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J42" t="str">
         <f t="shared" si="0"/>
-        <v>LR1F220K</v>
+        <v>LR1F390R</v>
       </c>
       <c r="K42">
         <f t="shared" si="1"/>
@@ -2833,33 +5183,33 @@
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B43">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C43" t="s">
-        <v>105</v>
+        <v>217</v>
       </c>
       <c r="D43" t="s">
         <v>79</v>
       </c>
       <c r="E43" t="s">
-        <v>82</v>
+        <v>100</v>
       </c>
       <c r="F43" t="s">
         <v>80</v>
       </c>
       <c r="H43" t="s">
-        <v>196</v>
+        <v>216</v>
       </c>
       <c r="J43" t="str">
         <f t="shared" si="0"/>
-        <v>LR1F390R</v>
+        <v>RR02J22KTB</v>
       </c>
       <c r="K43">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.2">
@@ -2867,57 +5217,57 @@
         <v>106</v>
       </c>
       <c r="B44">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C44" t="s">
-        <v>219</v>
+        <v>107</v>
       </c>
       <c r="D44" t="s">
         <v>79</v>
       </c>
       <c r="E44" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F44" t="s">
         <v>80</v>
       </c>
       <c r="H44" t="s">
-        <v>218</v>
+        <v>197</v>
       </c>
       <c r="J44" t="str">
         <f t="shared" si="0"/>
-        <v>RR02J22KTB</v>
+        <v>5083NW47K00JA100</v>
       </c>
       <c r="K44">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B45">
         <v>4</v>
       </c>
       <c r="C45" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D45" t="s">
         <v>79</v>
       </c>
       <c r="E45" t="s">
-        <v>101</v>
+        <v>82</v>
       </c>
       <c r="F45" t="s">
         <v>80</v>
       </c>
       <c r="H45" t="s">
-        <v>199</v>
+        <v>187</v>
       </c>
       <c r="J45" t="str">
         <f t="shared" si="0"/>
-        <v>5083NW47K00JA100</v>
+        <v>LR1F10R</v>
       </c>
       <c r="K45">
         <f t="shared" si="1"/>
@@ -2926,29 +5276,29 @@
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B46">
         <v>4</v>
       </c>
       <c r="C46" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D46" t="s">
         <v>79</v>
       </c>
       <c r="E46" t="s">
-        <v>82</v>
+        <v>100</v>
       </c>
       <c r="F46" t="s">
         <v>80</v>
       </c>
       <c r="H46" t="s">
-        <v>189</v>
+        <v>198</v>
       </c>
       <c r="J46" t="str">
         <f t="shared" si="0"/>
-        <v>LR1F10R</v>
+        <v>5083NW1K000J</v>
       </c>
       <c r="K46">
         <f t="shared" si="1"/>
@@ -2957,29 +5307,29 @@
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B47">
         <v>4</v>
       </c>
       <c r="C47" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D47" t="s">
         <v>79</v>
       </c>
       <c r="E47" t="s">
-        <v>101</v>
+        <v>82</v>
       </c>
       <c r="F47" t="s">
         <v>80</v>
       </c>
       <c r="H47" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="J47" t="str">
         <f t="shared" si="0"/>
-        <v>5083NW1K000J</v>
+        <v>LR1F270R</v>
       </c>
       <c r="K47">
         <f t="shared" si="1"/>
@@ -2988,218 +5338,193 @@
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B48">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C48" t="s">
-        <v>114</v>
+        <v>141</v>
       </c>
       <c r="D48" t="s">
         <v>79</v>
       </c>
       <c r="E48" t="s">
-        <v>82</v>
+        <v>100</v>
       </c>
       <c r="F48" t="s">
         <v>80</v>
       </c>
       <c r="H48" t="s">
-        <v>197</v>
+        <v>140</v>
       </c>
       <c r="J48" t="str">
         <f t="shared" si="0"/>
-        <v>LR1F270R</v>
+        <v>G00310R00FE7080</v>
       </c>
       <c r="K48">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>115</v>
+        <v>160</v>
       </c>
       <c r="B49">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C49" t="s">
-        <v>142</v>
+        <v>117</v>
       </c>
       <c r="D49" t="s">
-        <v>79</v>
+        <v>161</v>
       </c>
       <c r="E49" t="s">
-        <v>101</v>
+        <v>116</v>
       </c>
       <c r="F49" t="s">
-        <v>80</v>
+        <v>162</v>
       </c>
       <c r="H49" t="s">
-        <v>141</v>
+        <v>177</v>
       </c>
       <c r="J49" t="str">
         <f t="shared" si="0"/>
-        <v>G00310R00FE7080</v>
+        <v>3339P-1-503LF</v>
       </c>
       <c r="K49">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
+        <v>115</v>
+      </c>
+      <c r="B50">
+        <v>2</v>
+      </c>
+      <c r="C50" t="s">
+        <v>95</v>
+      </c>
+      <c r="D50" t="s">
+        <v>161</v>
+      </c>
+      <c r="E50" t="s">
+        <v>116</v>
+      </c>
+      <c r="F50" t="s">
         <v>162</v>
       </c>
-      <c r="B50">
-        <v>5</v>
-      </c>
-      <c r="C50" t="s">
-        <v>118</v>
-      </c>
-      <c r="D50" t="s">
-        <v>163</v>
-      </c>
-      <c r="E50" t="s">
-        <v>117</v>
-      </c>
-      <c r="F50" t="s">
-        <v>164</v>
-      </c>
       <c r="H50" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="J50" t="str">
         <f t="shared" si="0"/>
-        <v>3339P-1-503LF</v>
+        <v>3339P-1-501LF</v>
       </c>
       <c r="K50">
-        <f t="shared" si="1"/>
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
+        <v>168</v>
+      </c>
+      <c r="B51">
+        <v>2</v>
+      </c>
+      <c r="C51" t="s">
+        <v>97</v>
+      </c>
+      <c r="D51" t="s">
+        <v>161</v>
+      </c>
+      <c r="E51" t="s">
         <v>116</v>
       </c>
-      <c r="B51">
-        <v>2</v>
-      </c>
-      <c r="C51" t="s">
-        <v>96</v>
-      </c>
-      <c r="D51" t="s">
-        <v>163</v>
-      </c>
-      <c r="E51" t="s">
-        <v>117</v>
-      </c>
       <c r="F51" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="H51" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="J51" t="str">
         <f t="shared" si="0"/>
-        <v>3339P-1-501LF</v>
+        <v>3339P-1-102LF</v>
       </c>
       <c r="K51">
-        <v>3</v>
+        <f t="shared" si="1"/>
+        <v>2</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>170</v>
+        <v>118</v>
       </c>
       <c r="B52">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C52" t="s">
-        <v>98</v>
+        <v>119</v>
       </c>
       <c r="D52" t="s">
-        <v>163</v>
+        <v>120</v>
       </c>
       <c r="E52" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="F52" t="s">
-        <v>164</v>
+        <v>122</v>
       </c>
       <c r="H52" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="J52" t="str">
         <f t="shared" si="0"/>
-        <v>3339P-1-102LF</v>
+        <v>CL140</v>
       </c>
       <c r="K52">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="B53">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C53" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="D53" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="E53" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="F53" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="H53" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="J53" t="str">
         <f t="shared" si="0"/>
-        <v>CL140</v>
+        <v>5006</v>
       </c>
       <c r="K53">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
-        <v>124</v>
-      </c>
-      <c r="B54">
-        <v>10</v>
-      </c>
-      <c r="C54" t="s">
-        <v>125</v>
-      </c>
-      <c r="D54" t="s">
-        <v>125</v>
-      </c>
-      <c r="E54" t="s">
-        <v>126</v>
-      </c>
-      <c r="F54" t="s">
-        <v>127</v>
-      </c>
-      <c r="H54" t="s">
-        <v>183</v>
-      </c>
       <c r="J54" t="str">
         <f t="shared" si="0"/>
-        <v>5006</v>
-      </c>
-      <c r="K54">
-        <f t="shared" si="1"/>
-        <v>10</v>
+        <v/>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.2">
@@ -3221,6 +5546,9 @@
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>202</v>
+      </c>
       <c r="J58" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3228,33 +5556,43 @@
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>204</v>
+        <v>203</v>
+      </c>
+      <c r="B59">
+        <v>1</v>
+      </c>
+      <c r="H59" t="s">
+        <v>212</v>
+      </c>
+      <c r="I59" t="s">
+        <v>220</v>
       </c>
       <c r="J59" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>LXH387USBD-150</v>
+      </c>
+      <c r="K59">
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
+        <v>204</v>
+      </c>
+      <c r="B60">
+        <v>2</v>
+      </c>
+      <c r="H60" t="s">
         <v>205</v>
       </c>
-      <c r="B60">
-        <v>1</v>
-      </c>
-      <c r="H60" t="s">
-        <v>214</v>
-      </c>
-      <c r="I60" t="s">
-        <v>222</v>
-      </c>
       <c r="J60" t="str">
         <f t="shared" si="0"/>
-        <v>LXH387USBD-150</v>
+        <v>6883</v>
       </c>
       <c r="K60">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.2">
@@ -3262,18 +5600,18 @@
         <v>206</v>
       </c>
       <c r="B61">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H61" t="s">
         <v>207</v>
       </c>
       <c r="J61" t="str">
         <f t="shared" si="0"/>
-        <v>6883</v>
+        <v>NYS367-2</v>
       </c>
       <c r="K61">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.2">
@@ -3288,7 +5626,7 @@
       </c>
       <c r="J62" t="str">
         <f t="shared" si="0"/>
-        <v>NYS367-2</v>
+        <v>NYS367-0</v>
       </c>
       <c r="K62">
         <f t="shared" si="1"/>
@@ -3307,7 +5645,7 @@
       </c>
       <c r="J63" t="str">
         <f t="shared" si="0"/>
-        <v>NYS367-0</v>
+        <v>4304.6090</v>
       </c>
       <c r="K63">
         <f t="shared" si="1"/>
@@ -3316,498 +5654,32 @@
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B64">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H64" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="J64" t="str">
         <f t="shared" si="0"/>
-        <v>4304.6090</v>
+        <v>745</v>
       </c>
       <c r="K64">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>215</v>
       </c>
-      <c r="B65">
-        <v>4</v>
-      </c>
-      <c r="H65" t="s">
-        <v>216</v>
-      </c>
-      <c r="J65" t="str">
-        <f t="shared" si="0"/>
-        <v>745</v>
-      </c>
-      <c r="K65">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
-        <v>217</v>
-      </c>
-      <c r="I66" t="s">
-        <v>223</v>
+      <c r="I65" t="s">
+        <v>221</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B270E01A-C831-5B46-99F7-CEE7B1F93A2B}">
-  <dimension ref="A1:B54"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>224</v>
-      </c>
-      <c r="B1" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>201</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>128</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>129</v>
-      </c>
-      <c r="B4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>130</v>
-      </c>
-      <c r="B5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>132</v>
-      </c>
-      <c r="B6">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>135</v>
-      </c>
-      <c r="B7">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>131</v>
-      </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>133</v>
-      </c>
-      <c r="B9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>134</v>
-      </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>136</v>
-      </c>
-      <c r="B11">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>137</v>
-      </c>
-      <c r="B12">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>138</v>
-      </c>
-      <c r="B13">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>139</v>
-      </c>
-      <c r="B14">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>203</v>
-      </c>
-      <c r="B15">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>178</v>
-      </c>
-      <c r="B16">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>176</v>
-      </c>
-      <c r="B17">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>220</v>
-      </c>
-      <c r="B18">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>175</v>
-      </c>
-      <c r="B19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>174</v>
-      </c>
-      <c r="B20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>173</v>
-      </c>
-      <c r="B21">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>172</v>
-      </c>
-      <c r="B22">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>140</v>
-      </c>
-      <c r="B23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>184</v>
-      </c>
-      <c r="B24">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>185</v>
-      </c>
-      <c r="B25">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>186</v>
-      </c>
-      <c r="B26">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>187</v>
-      </c>
-      <c r="B27">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>188</v>
-      </c>
-      <c r="B28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>189</v>
-      </c>
-      <c r="B29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>190</v>
-      </c>
-      <c r="B30">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>191</v>
-      </c>
-      <c r="B31">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>192</v>
-      </c>
-      <c r="B32">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>193</v>
-      </c>
-      <c r="B33">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>194</v>
-      </c>
-      <c r="B34">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>198</v>
-      </c>
-      <c r="B35">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>195</v>
-      </c>
-      <c r="B36">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>196</v>
-      </c>
-      <c r="B37">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>218</v>
-      </c>
-      <c r="B38">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>199</v>
-      </c>
-      <c r="B39">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>189</v>
-      </c>
-      <c r="B40">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>200</v>
-      </c>
-      <c r="B41">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
-        <v>197</v>
-      </c>
-      <c r="B42">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
-        <v>141</v>
-      </c>
-      <c r="B43">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
-        <v>179</v>
-      </c>
-      <c r="B44">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
-        <v>180</v>
-      </c>
-      <c r="B45">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
-        <v>181</v>
-      </c>
-      <c r="B46">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
-        <v>182</v>
-      </c>
-      <c r="B47">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
-        <v>183</v>
-      </c>
-      <c r="B48">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
-        <v>214</v>
-      </c>
-      <c r="B49">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
-        <v>207</v>
-      </c>
-      <c r="B50">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
-        <v>209</v>
-      </c>
-      <c r="B51">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
-        <v>211</v>
-      </c>
-      <c r="B52">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
-        <v>213</v>
-      </c>
-      <c r="B53">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
-        <v>216</v>
-      </c>
-      <c r="B54">
-        <v>4</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>